<commit_message>
Progress on two_body_utils.py and two_body.ipynb
</commit_message>
<xml_diff>
--- a/Omega Centauri Data.xlsx
+++ b/Omega Centauri Data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smuhalifax-my.sharepoint.com/personal/mackenzie_hayduk_smu_ca/Documents/Summer Research 2025/two_body/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{9C30D00F-EE86-4F7B-943B-56E14CD88756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{166B60DC-354A-4F3C-96C2-BFA9FE3884A7}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="8_{9C30D00F-EE86-4F7B-943B-56E14CD88756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A86A430-3B6D-4BBD-8C77-8F6087B7D572}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{7A33FF95-5BB8-4AF8-A869-0852F0F74D25}"/>
+    <workbookView minimized="1" xWindow="1725" yWindow="1725" windowWidth="7500" windowHeight="6000" activeTab="1" xr2:uid="{7A33FF95-5BB8-4AF8-A869-0852F0F74D25}"/>
   </bookViews>
   <sheets>
     <sheet name="v2D and a_mag" sheetId="1" r:id="rId1"/>
     <sheet name="Assumptions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>v2D</t>
   </si>
@@ -120,40 +121,37 @@
     <t>m_primary = 8200*M_SUN</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>m2m1</t>
-  </si>
-  <si>
-    <t>tau</t>
-  </si>
-  <si>
-    <t>mtot</t>
-  </si>
-  <si>
-    <t>per</t>
-  </si>
-  <si>
-    <t>Omega</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>nu</t>
-  </si>
-  <si>
-    <t>distance_kpc = 5.43 * u.kpc  distance_km = distance_kpc.to(u.km)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a </t>
+    <t xml:space="preserve">distance_kpc = 5.43 * u.kpc  </t>
+  </si>
+  <si>
+    <t>r_proj_starA = 0.265"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">angular distance from central mass for the two highest velocity stars </t>
+  </si>
+  <si>
+    <t>lower limit esitmate for central mass</t>
+  </si>
+  <si>
+    <t>distance of omega centauri from earth</t>
+  </si>
+  <si>
+    <t>r_proj_starC = 0.870"</t>
+  </si>
+  <si>
+    <t>v_2D_starA = 113.0 km/s</t>
+  </si>
+  <si>
+    <t>v_2D_starC = 94.9 km/s</t>
+  </si>
+  <si>
+    <t>2D velocities for the two highest velocity stars</t>
+  </si>
+  <si>
+    <t>Approximate average = 0.5"</t>
+  </si>
+  <si>
+    <t>Approximate average = 100 km/s</t>
   </si>
 </sst>
 </file>
@@ -213,17 +211,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,10 +590,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -685,14 +695,14 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -926,22 +936,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80C6ED7-958E-4ACE-93C9-1A63DD8C9A78}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="56.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>21</v>
       </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -950,9 +965,6 @@
       <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -961,63 +973,66 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D3" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
+      <c r="C8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>36</v>
-      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>